<commit_message>
more tests and change code
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Tests/Data/Template_L&T_test.xlsx
+++ b/Projects/CCBZA_SAND/Tests/Data/Template_L&T_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="175">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -231,13 +231,13 @@
     <t xml:space="preserve">size</t>
   </si>
   <si>
-    <t xml:space="preserve">brand</t>
+    <t xml:space="preserve">brand_name</t>
   </si>
   <si>
     <t xml:space="preserve">FANTA ORANGE, COCA COLA, SPRITE, STONEY</t>
   </si>
   <si>
-    <t xml:space="preserve">Container Type</t>
+    <t xml:space="preserve">form_factor</t>
   </si>
   <si>
     <t xml:space="preserve">can</t>
@@ -540,10 +540,16 @@
     <t xml:space="preserve">Min 4 x Cooler Doors</t>
   </si>
   <si>
+    <t xml:space="preserve">at least one cooler with 4 doors</t>
+  </si>
+  <si>
     <t xml:space="preserve">Min 3 x Cooler Doors</t>
   </si>
   <si>
     <t xml:space="preserve">Min 1 x Cooler Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one cooler with 3 doors?</t>
   </si>
 </sst>
 </file>
@@ -798,22 +804,22 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.6279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.9348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="41.2279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="21.7813953488372"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="19.9348837209302"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.4558139534884"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="22.3953488372093"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1131,26 +1137,26 @@
   </sheetPr>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="74.0837209302326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.5209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.293023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.4604651162791"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="47.9953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.4883720930233"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="55.0093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="76.2976744186047"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3813953488372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5348837209302"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.953488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.4697674418605"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8883720930233"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="56.6093023255814"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1726,20 +1732,20 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="44.4604651162791"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.2093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4883720930233"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.7813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7348837209302"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6139534883721"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.706976744186"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2579,28 +2585,27 @@
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M12" activeCellId="0" sqref="M12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="83.9302325581395"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.9023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="48.8558139534884"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.4279069767442"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="86.3906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5488372093023"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.3302325581395"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6744186046512"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.27441860465116"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.4883720930233"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="66.4558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.4"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="68.5441860465116"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3164,28 +3169,28 @@
   </sheetPr>
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N1" activeCellId="0" sqref="N1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="102.879069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.2418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3023255813953"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="24.8604651162791"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="30.5209302325581"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.106976744186"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.2744186046512"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.2"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="105.958139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6604651162791"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="25.5953488372093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.3813953488372"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8418604651163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.1348837209302"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8139534883721"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3602,22 +3607,22 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.84651162790698"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3671,6 +3676,9 @@
       <c r="H2" s="0" t="s">
         <v>100</v>
       </c>
+      <c r="I2" s="0" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="17" t="s">
@@ -3680,7 +3688,7 @@
         <v>53</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
@@ -3706,7 +3714,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -3723,6 +3731,9 @@
       <c r="H4" s="0" t="s">
         <v>97</v>
       </c>
+      <c r="I4" s="0" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="17" t="s">
@@ -3750,7 +3761,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
@@ -3758,7 +3769,7 @@
         <v>53</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
@@ -3784,7 +3795,7 @@
         <v>53</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -3836,7 +3847,7 @@
         <v>53</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>3</v>
@@ -3862,7 +3873,7 @@
         <v>53</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -3914,7 +3925,7 @@
         <v>53</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>3</v>
@@ -3940,7 +3951,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -3992,7 +4003,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>3</v>
@@ -4018,7 +4029,7 @@
         <v>53</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
@@ -4070,7 +4081,7 @@
         <v>53</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>3</v>
@@ -4096,7 +4107,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
refactoring code and tests
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Tests/Data/Template_L&T_test.xlsx
+++ b/Projects/CCBZA_SAND/Tests/Data/Template_L&T_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="176">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -498,7 +498,7 @@
     <t xml:space="preserve">Quad Cola</t>
   </si>
   <si>
-    <t xml:space="preserve">Attribute 2 </t>
+    <t xml:space="preserve">Attribute 2</t>
   </si>
   <si>
     <t xml:space="preserve">SSD</t>
@@ -510,10 +510,13 @@
     <t xml:space="preserve">Diets</t>
   </si>
   <si>
+    <t xml:space="preserve">Attribute 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spaza Affordable </t>
+  </si>
+  <si>
     <t xml:space="preserve">Attribute 3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spaza Affordable </t>
   </si>
   <si>
     <t xml:space="preserve">"dealer owned" cooler with SOVI &gt; 50% in Energy &amp; SOVI &gt; 35% in Water catgeory, with pricing communication.</t>
@@ -804,22 +807,22 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.7348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.1162790697674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.9209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="42.4558139534884"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.0418604651163"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="22.3953488372093"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.3488372093023"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.9023255813953"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.6883720930233"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5348837209302"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="23.0139534883721"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,29 +1140,29 @@
   </sheetPr>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4418604651163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="76.2976744186047"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.3813953488372"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5348837209302"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.953488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="49.4697674418605"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8883720930233"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="56.6093023255814"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0604651162791"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.6604651162791"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.906976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9348837209302"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.9488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2604651162791"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="58.3302325581395"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1411,7 +1414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="s">
         <v>16</v>
       </c>
@@ -1449,7 +1452,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
@@ -1479,7 +1482,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
@@ -1499,7 +1502,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
         <v>16</v>
       </c>
@@ -1519,7 +1522,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="s">
         <v>19</v>
       </c>
@@ -1539,7 +1542,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
@@ -1559,7 +1562,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
         <v>20</v>
       </c>
@@ -1599,7 +1602,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
         <v>20</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
         <v>21</v>
       </c>
@@ -1639,7 +1642,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>22</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="57" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>27</v>
       </c>
@@ -1688,7 +1691,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>27</v>
       </c>
@@ -1737,15 +1740,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.7813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.7348837209302"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.6139534883721"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.706976744186"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.106976744186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2585,27 +2588,28 @@
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="86.3906976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.7674418604651"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.5488372093023"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.3302325581395"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.6744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="88.9720930232558"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.6279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.8093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9209302325581"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.86046511627907"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.76744186046512"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.4"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="68.5441860465116"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.89302325581395"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.52093023255814"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="70.5162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3170,27 +3174,27 @@
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="105.958139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.6604651162791"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9813953488372"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.0418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="31.3813953488372"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="25.8418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.1348837209302"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.8139534883721"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="109.158139534884"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7209302325581"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="26.3348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.9953488372093"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.2418604651163"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.5813953488372"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.9953488372093"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.4279069767442"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3246,7 +3250,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
@@ -3296,7 +3300,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -3325,7 +3329,7 @@
         <v>160</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K3" s="0" t="s">
         <v>158</v>
@@ -3346,7 +3350,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
@@ -3375,7 +3379,7 @@
         <v>160</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K4" s="0" t="s">
         <v>158</v>
@@ -3396,7 +3400,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
@@ -3425,7 +3429,7 @@
         <v>160</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>158</v>
@@ -3446,7 +3450,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
@@ -3475,7 +3479,7 @@
         <v>160</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>158</v>
@@ -3496,7 +3500,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
@@ -3525,7 +3529,7 @@
         <v>160</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K7" s="0" t="s">
         <v>158</v>
@@ -3551,19 +3555,19 @@
         <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>159</v>
@@ -3572,13 +3576,13 @@
         <v>50</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>159</v>
@@ -3610,19 +3614,19 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.5488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.84651162790698"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.84651162790698"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4744186046512"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.093023255814"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3659,7 +3663,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>4</v>
@@ -3677,7 +3681,7 @@
         <v>100</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3688,7 +3692,7 @@
         <v>53</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
@@ -3714,7 +3718,7 @@
         <v>53</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -3732,7 +3736,7 @@
         <v>97</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3743,7 +3747,7 @@
         <v>53</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -3769,7 +3773,7 @@
         <v>53</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
@@ -3795,7 +3799,7 @@
         <v>53</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -3821,7 +3825,7 @@
         <v>53</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>4</v>
@@ -3847,7 +3851,7 @@
         <v>53</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>3</v>
@@ -3873,7 +3877,7 @@
         <v>53</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -3899,7 +3903,7 @@
         <v>53</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>4</v>
@@ -3925,7 +3929,7 @@
         <v>53</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>3</v>
@@ -3951,7 +3955,7 @@
         <v>53</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -3977,7 +3981,7 @@
         <v>53</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>4</v>
@@ -4003,7 +4007,7 @@
         <v>53</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>3</v>
@@ -4029,7 +4033,7 @@
         <v>53</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
@@ -4055,7 +4059,7 @@
         <v>53</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>4</v>
@@ -4081,7 +4085,7 @@
         <v>53</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>3</v>
@@ -4107,7 +4111,7 @@
         <v>53</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
the tests, adding planogram function tologic
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Tests/Data/Template_L&T_test.xlsx
+++ b/Projects/CCBZA_SAND/Tests/Data/Template_L&T_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="Availability" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="SOS" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Count" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Planogram" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="182">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -553,6 +554,24 @@
   </si>
   <si>
     <t xml:space="preserve">one cooler with 3 doors?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Template Display Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merchandising</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooler Merchandised as per planogram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Door Cooler, 3 Door Cooler, 2 Door Cooler, 1 Door Cooler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least one template should pass the planogram for this KPI to pass</t>
   </si>
 </sst>
 </file>
@@ -655,7 +674,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -725,6 +744,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -813,16 +836,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="41.9627906976744"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.3488372093023"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.9023255813953"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="43.6883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5348837209302"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="23.0139534883721"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.1953488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5813953488372"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.0093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.0418604651163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.153488372093"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="23.6279069767442"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1140,26 +1163,26 @@
   </sheetPr>
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O13" activeCellId="0" sqref="O13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0604651162791"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="69.6604651162791"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.2418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.906976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="50.9488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.4744186046512"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="58.3302325581395"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.553488372093"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.7441860465116"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2744186046512"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.5488372093023"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6279069767442"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="60.0558139534884"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1740,15 +1763,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1348837209302"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.2279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.106976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.4883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7209302325581"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2594,22 +2617,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="88.9720930232558"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.6279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.2883720930233"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.8093023255814"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.9209302325581"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.6790697674419"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.0279069767442"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.2837209302326"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1674418604651"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.10697674418605"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="6.89302325581395"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.52093023255814"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.4744186046512"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.093023255814"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="70.5162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="7.01395348837209"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.64651162790698"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="72.6046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3179,22 +3202,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="109.158139534884"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.2744186046512"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="25.7209302325581"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="26.3348837209302"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.9953488372093"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.2418604651163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="26.5813953488372"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="31.9953488372093"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.01395348837209"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.0883720930233"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="112.479069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8883720930233"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.4604651162791"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.0744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7348837209302"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.2279069767442"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.4418604651163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="32.9813953488372"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.9209302325581"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5813953488372"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,14 +3642,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.2883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.093023255814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.4744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.093023255814"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.0279069767442"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.9674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3395348837209"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4138,4 +4161,91 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <tabColor rgb="FFFFC000"/>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5953488372093"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.1767441860465"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.72093023255814"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="59.3162790697674"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86046511627907"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding code, changing template, adding tests
</commit_message>
<xml_diff>
--- a/Projects/CCBZA_SAND/Tests/Data/Template_L&T_test.xlsx
+++ b/Projects/CCBZA_SAND/Tests/Data/Template_L&T_test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="KPI" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="184">
   <si>
     <t xml:space="preserve">Set Name</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t xml:space="preserve">Attribute_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By Scene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KO Only</t>
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
@@ -727,6 +733,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -744,10 +754,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -830,22 +836,22 @@
   </sheetPr>
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="43.1953488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.5813953488372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="39.0093023255814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="45.0418604651163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.153488372093"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="23.6279069767442"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="21.4139534883721"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.5488372093023"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.9348837209302"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.1162790697674"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="46.2697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.7674418604651"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="24.2418604651163"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="22.0279069767442"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1161,28 +1167,30 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M26" activeCellId="0" sqref="M26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.553488372093"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="71.7441860465116"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.2279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.2744186046512"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.1813953488372"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="52.5488372093023"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="7.01395348837209"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="60.0558139534884"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.0418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="73.8372093023256"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.2093023255814"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.646511627907"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.6744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4279069767442"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="54.0232558139535"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16"/>
+    <col collapsed="false" hidden="false" max="11" min="9" style="0" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="9.6"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="12.8"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="61.7767441860465"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1231,40 +1239,52 @@
       <c r="O1" s="5" t="s">
         <v>51</v>
       </c>
+      <c r="P1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>60</v>
+        <v>61</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1272,34 +1292,40 @@
         <v>12</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>4</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1307,34 +1333,40 @@
         <v>12</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>5</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M4" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1342,34 +1374,40 @@
         <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>4</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>60</v>
+        <v>65</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1377,34 +1415,40 @@
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>4</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>60</v>
+        <v>66</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1412,29 +1456,35 @@
         <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="L7" s="8"/>
       <c r="M7" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="O7" s="7" t="s">
-        <v>60</v>
+        <v>67</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1442,37 +1492,43 @@
         <v>16</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E8" s="9" t="n">
         <v>200</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>5</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O8" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,13 +1536,13 @@
         <v>16</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
@@ -1496,13 +1552,19 @@
         <v>5</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O9" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1510,19 +1572,25 @@
         <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1530,19 +1598,25 @@
         <v>16</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,19 +1624,25 @@
         <v>19</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>5</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,19 +1650,25 @@
         <v>19</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J13" s="0" t="n">
         <v>7</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,19 +1676,25 @@
         <v>19</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J14" s="0" t="n">
         <v>9</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q14" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1610,19 +1702,25 @@
         <v>20</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J15" s="0" t="n">
         <v>13</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1630,19 +1728,25 @@
         <v>20</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J16" s="0" t="n">
         <v>10.5</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O16" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1650,19 +1754,25 @@
         <v>21</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J17" s="0" t="n">
         <v>12.99</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q17" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,19 +1780,25 @@
         <v>22</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="J18" s="0" t="n">
         <v>10</v>
       </c>
       <c r="L18" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O18" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1690,13 +1806,13 @@
         <v>27</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="J19" s="0" t="n">
         <v>14</v>
@@ -1705,13 +1821,19 @@
         <v>3</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M19" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1719,7 +1841,7 @@
         <v>27</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="E20" s="12"/>
       <c r="J20" s="0" t="n">
@@ -1729,13 +1851,19 @@
         <v>3</v>
       </c>
       <c r="L20" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M20" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>72</v>
+        <v>61</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="P20" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1757,21 +1885,21 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="48.4883720930233"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.7209302325581"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.446511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.9627906976744"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.2139534883721"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.8139534883721"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1782,10 +1910,10 @@
         <v>38</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>47</v>
@@ -1805,10 +1933,10 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" s="7" t="n">
         <v>21</v>
@@ -1817,10 +1945,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,10 +1956,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D3" s="7" t="n">
         <v>22</v>
@@ -1840,10 +1968,10 @@
         <v>15</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1851,10 +1979,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>23</v>
@@ -1863,10 +1991,10 @@
         <v>10</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1874,10 +2002,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D5" s="7" t="n">
         <v>24</v>
@@ -1886,10 +2014,10 @@
         <v>13</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1897,10 +2025,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D6" s="7" t="n">
         <v>25</v>
@@ -1909,10 +2037,10 @@
         <v>10</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1920,10 +2048,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D7" s="7" t="n">
         <v>26</v>
@@ -1932,10 +2060,10 @@
         <v>13</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1943,19 +2071,19 @@
         <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>87</v>
       </c>
       <c r="D8" s="7" t="n">
         <v>27</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1963,19 +2091,19 @@
         <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>87</v>
       </c>
       <c r="D9" s="7" t="n">
         <v>28</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1983,19 +2111,19 @@
         <v>20</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>87</v>
       </c>
       <c r="D10" s="7" t="n">
         <v>29</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2003,19 +2131,19 @@
         <v>21</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>87</v>
       </c>
       <c r="D11" s="7" t="n">
         <v>30</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,19 +2151,19 @@
         <v>22</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D12" s="7" t="n">
         <v>31</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2043,10 +2171,10 @@
         <v>30</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D13" s="7" t="n">
         <v>32</v>
@@ -2055,10 +2183,10 @@
         <v>3</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2066,10 +2194,10 @@
         <v>30</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D14" s="7" t="n">
         <v>33</v>
@@ -2078,10 +2206,10 @@
         <v>3</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2089,10 +2217,10 @@
         <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D15" s="7" t="n">
         <v>34</v>
@@ -2101,10 +2229,10 @@
         <v>3</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2112,10 +2240,10 @@
         <v>30</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D16" s="7" t="n">
         <v>35</v>
@@ -2124,10 +2252,10 @@
         <v>3</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2135,10 +2263,10 @@
         <v>37</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D17" s="7" t="n">
         <v>1</v>
@@ -2147,7 +2275,7 @@
         <v>5</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2155,10 +2283,10 @@
         <v>37</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D18" s="7" t="n">
         <v>2</v>
@@ -2167,10 +2295,10 @@
         <v>10</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2178,10 +2306,10 @@
         <v>37</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D19" s="7" t="n">
         <v>3</v>
@@ -2190,10 +2318,10 @@
         <v>15</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2201,10 +2329,10 @@
         <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D20" s="7" t="n">
         <v>4</v>
@@ -2213,10 +2341,10 @@
         <v>3</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,10 +2352,10 @@
         <v>37</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D21" s="7" t="n">
         <v>5</v>
@@ -2236,10 +2364,10 @@
         <v>4</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2247,10 +2375,10 @@
         <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D22" s="7" t="n">
         <v>6</v>
@@ -2259,10 +2387,10 @@
         <v>2</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2270,10 +2398,10 @@
         <v>37</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D23" s="7" t="n">
         <v>7</v>
@@ -2282,13 +2410,13 @@
         <v>12</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2296,10 +2424,10 @@
         <v>37</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D24" s="7" t="n">
         <v>8</v>
@@ -2308,10 +2436,10 @@
         <v>7</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2319,10 +2447,10 @@
         <v>37</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D25" s="7" t="n">
         <v>9</v>
@@ -2331,13 +2459,13 @@
         <v>9</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,10 +2473,10 @@
         <v>37</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D26" s="7" t="n">
         <v>10</v>
@@ -2357,10 +2485,10 @@
         <v>14</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2368,10 +2496,10 @@
         <v>37</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D27" s="7" t="n">
         <v>11</v>
@@ -2380,7 +2508,7 @@
         <v>13</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2388,10 +2516,10 @@
         <v>37</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D28" s="7" t="n">
         <v>12</v>
@@ -2400,13 +2528,13 @@
         <v>5</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2414,10 +2542,10 @@
         <v>37</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D29" s="7" t="n">
         <v>13</v>
@@ -2426,10 +2554,10 @@
         <v>4</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2437,10 +2565,10 @@
         <v>37</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D30" s="7" t="n">
         <v>14</v>
@@ -2449,13 +2577,13 @@
         <v>10</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,10 +2591,10 @@
         <v>37</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D31" s="7" t="n">
         <v>15</v>
@@ -2475,10 +2603,10 @@
         <v>11</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2486,10 +2614,10 @@
         <v>37</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D32" s="7" t="n">
         <v>16</v>
@@ -2498,13 +2626,13 @@
         <v>16</v>
       </c>
       <c r="F32" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="G32" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="H32" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2512,10 +2640,10 @@
         <v>37</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D33" s="7" t="n">
         <v>17</v>
@@ -2524,10 +2652,10 @@
         <v>2</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2535,10 +2663,10 @@
         <v>37</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D34" s="7" t="n">
         <v>18</v>
@@ -2547,13 +2675,13 @@
         <v>7</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2609,33 +2737,35 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P22" activeCellId="0" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.646511627907"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="91.6790697674419"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.4883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.0279069767442"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="53.2837209302326"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.0139534883721"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="94.3906976744186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.4744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.8883720930233"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="54.8837209302326"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.4139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.35348837209302"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.29302325581395"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="7.01395348837209"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.64651162790698"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="72.6046511627907"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="0" width="7.13953488372093"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="6.76744186046512"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.5906976744186"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="12.5255813953488"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="74.8232558139535"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -2643,7 +2773,7 @@
         <v>38</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>39</v>
@@ -2684,28 +2814,34 @@
       <c r="P1" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Q1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -2717,32 +2853,38 @@
         <v>2</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K3" s="0" t="n">
         <v>2</v>
@@ -2751,33 +2893,39 @@
         <v>5</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="P3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K4" s="0" t="n">
         <v>2</v>
@@ -2786,33 +2934,39 @@
         <v>4</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+      <c r="P4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K5" s="0" t="n">
         <v>2</v>
@@ -2821,33 +2975,39 @@
         <v>4</v>
       </c>
       <c r="M5" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N5" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>64</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K6" s="0" t="n">
         <v>2</v>
@@ -2856,33 +3016,39 @@
         <v>3</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>65</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K7" s="0" t="n">
         <v>2</v>
@@ -2891,33 +3057,39 @@
         <v>4</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="K8" s="0" t="n">
         <v>2</v>
@@ -2926,255 +3098,321 @@
         <v>3</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" s="7" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" s="7" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>130</v>
+        <v>76</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="K9" s="7" t="n">
         <v>2</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="P9" s="14" t="s">
-        <v>131</v>
+        <v>61</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" s="7" customFormat="true" ht="42.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="R9" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" s="7" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F10" s="13"/>
+        <v>76</v>
+      </c>
+      <c r="F10" s="14"/>
       <c r="K10" s="7" t="n">
         <v>2</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="P10" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="R10" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="Q10" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>129</v>
-      </c>
       <c r="D11" s="7"/>
-      <c r="F11" s="13"/>
+      <c r="F11" s="14"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
-      <c r="P11" s="14"/>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R11" s="15"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="7" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D12" s="7"/>
-      <c r="F12" s="13"/>
+      <c r="F12" s="14"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="P12" s="14"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>135</v>
+        <v>76</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="K13" s="0" t="n">
         <v>2</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q13" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="P13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="S13" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>137</v>
+        <v>76</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>139</v>
       </c>
       <c r="K14" s="0" t="n">
         <v>3</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q14" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="P14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
         <v>20</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E15" s="7"/>
       <c r="K15" s="0" t="n">
         <v>2</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="P15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
         <v>21</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K16" s="0" t="n">
         <v>2</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="P16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q16" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>22</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K17" s="0" t="n">
         <v>2</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>61</v>
+      </c>
+      <c r="P17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q17" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
         <v>24</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K18" s="0" t="n">
         <v>2</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="P18" s="7" t="s">
-        <v>142</v>
+        <v>61</v>
+      </c>
+      <c r="P18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3194,33 +3432,33 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M30" activeCellId="0" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="112.479069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.8883720930233"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.4604651162791"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.6418604651163"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.0744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="24.7348837209302"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.2279069767442"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="32.9813953488372"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="20.9209302325581"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.13953488372093"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="18.5813953488372"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="115.925581395349"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.506976744186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.1953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.5023255813953"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="27.9348837209302"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.4744186046512"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="34.2093023255814"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.3023255813953"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="33.9674418604651"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="21.4139534883721"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.26046511627907"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="19.2"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -3231,37 +3469,37 @@
         <v>39</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>48</v>
@@ -3271,6 +3509,12 @@
       </c>
       <c r="Q1" s="6" t="s">
         <v>50</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3278,37 +3522,37 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H2" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I2" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="K2" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="L2" s="0" t="s">
         <v>161</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" s="0" t="s">
-        <v>159</v>
       </c>
       <c r="M2" s="0" t="n">
         <v>30</v>
@@ -3317,10 +3561,16 @@
         <v>5</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>162</v>
+        <v>164</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3328,37 +3578,37 @@
         <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I3" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="K3" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="J3" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="L3" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M3" s="0" t="n">
         <v>30</v>
@@ -3367,10 +3617,16 @@
         <v>4</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3378,37 +3634,37 @@
         <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H4" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I4" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="J4" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="L4" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M4" s="0" t="n">
         <v>30</v>
@@ -3417,10 +3673,16 @@
         <v>4</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>62</v>
+        <v>64</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3428,37 +3690,37 @@
         <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H5" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I5" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="J5" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="L5" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M5" s="0" t="n">
         <v>30</v>
@@ -3467,10 +3729,16 @@
         <v>3</v>
       </c>
       <c r="O5" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3478,37 +3746,37 @@
         <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H6" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I6" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="K6" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="J6" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="L6" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M6" s="0" t="n">
         <v>30</v>
@@ -3517,10 +3785,16 @@
         <v>4</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>64</v>
+        <v>66</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S6" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3528,37 +3802,37 @@
         <v>12</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H7" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I7" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="K7" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="J7" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>158</v>
-      </c>
       <c r="L7" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M7" s="0" t="n">
         <v>30</v>
@@ -3567,10 +3841,16 @@
         <v>3</v>
       </c>
       <c r="O7" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>65</v>
+        <v>67</v>
+      </c>
+      <c r="R7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S7" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3578,43 +3858,49 @@
         <v>34</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H8" s="0" t="n">
         <v>50</v>
       </c>
       <c r="I8" s="0" t="s">
+        <v>171</v>
+      </c>
+      <c r="J8" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="J8" s="0" t="s">
-        <v>167</v>
-      </c>
       <c r="K8" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="M8" s="0" t="n">
         <v>35</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
+      </c>
+      <c r="R8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="S8" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -3634,39 +3920,39 @@
     <tabColor rgb="FFFFC000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.0279069767442"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3395348837209"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7674418604651"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8139534883721"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.9674418604651"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.3395348837209"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.8883720930233"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6418604651163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5813953488372"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3813953488372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.1813953488372"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.4604651162791"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.5813953488372"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>38</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>48</v>
@@ -3677,16 +3963,22 @@
       <c r="H1" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
+      <c r="I1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>171</v>
+      <c r="B2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>4</v>
@@ -3695,27 +3987,33 @@
         <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>173</v>
+      <c r="B3" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>3</v>
@@ -3724,24 +4022,30 @@
         <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>174</v>
+      <c r="B4" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>176</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -3750,27 +4054,33 @@
         <v>10</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>171</v>
+      <c r="B5" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>4</v>
@@ -3779,24 +4089,30 @@
         <v>6</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>173</v>
+      <c r="B6" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>3</v>
@@ -3805,24 +4121,30 @@
         <v>6</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>174</v>
+      <c r="B7" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>176</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -3831,24 +4153,30 @@
         <v>6</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>171</v>
+      <c r="B8" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>4</v>
@@ -3857,24 +4185,30 @@
         <v>8</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>173</v>
+      <c r="B9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>3</v>
@@ -3883,24 +4217,30 @@
         <v>8</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>174</v>
+      <c r="B10" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>176</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -3909,24 +4249,30 @@
         <v>8</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>171</v>
+      <c r="B11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>4</v>
@@ -3935,24 +4281,30 @@
         <v>6</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>173</v>
+      <c r="B12" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="D12" s="0" t="n">
         <v>3</v>
@@ -3961,24 +4313,30 @@
         <v>6</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>174</v>
+      <c r="B13" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>176</v>
       </c>
       <c r="D13" s="0" t="n">
         <v>1</v>
@@ -3987,24 +4345,30 @@
         <v>6</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>171</v>
+      <c r="B14" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>4</v>
@@ -4013,24 +4377,30 @@
         <v>8</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>173</v>
+      <c r="B15" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>3</v>
@@ -4039,24 +4409,30 @@
         <v>8</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>174</v>
+      <c r="B16" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>176</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>1</v>
@@ -4065,24 +4441,30 @@
         <v>8</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I16" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>171</v>
+      <c r="B17" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>173</v>
       </c>
       <c r="D17" s="0" t="n">
         <v>4</v>
@@ -4091,24 +4473,30 @@
         <v>6</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>173</v>
+      <c r="B18" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>175</v>
       </c>
       <c r="D18" s="0" t="n">
         <v>3</v>
@@ -4117,24 +4505,30 @@
         <v>6</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>174</v>
+      <c r="B19" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>176</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>1</v>
@@ -4143,13 +4537,19 @@
         <v>6</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+      <c r="I19" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -4171,20 +4571,20 @@
   </sheetPr>
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="58" zoomScaleNormal="58" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="49.5953488372093"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="52.1767441860465"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.86046511627907"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.96744186046512"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.72093023255814"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="59.3162790697674"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.6744186046512"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="51.0697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="53.6558139534884"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.2139534883721"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.96744186046512"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="61.1627906976744"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4195,13 +4595,13 @@
         <v>38</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>48</v>
@@ -4213,18 +4613,18 @@
         <v>50</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>100</v>
@@ -4232,11 +4632,11 @@
       <c r="E2" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>109</v>
+      <c r="F2" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>